<commit_message>
3,5 position x, y add
</commit_message>
<xml_diff>
--- a/demo/src/data/SubwayInfoList.xlsx
+++ b/demo/src/data/SubwayInfoList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\react_nodeExpress\demo\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC3DFA8-CE89-44A3-AAF0-CB487A77CC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6132E03-0A9E-4347-9D39-7D037973A7B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3360" yWindow="615" windowWidth="25140" windowHeight="16410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29460" yWindow="810" windowWidth="25140" windowHeight="16410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="서울시 지하철역 정보 검색 (역명)" sheetId="1" r:id="rId1"/>
@@ -3930,8 +3930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D768"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>